<commit_message>
change to tropo tau
</commit_message>
<xml_diff>
--- a/get_tts/tts_per_rf/tts_per_rf_figs/Comparison_Table.xlsx
+++ b/get_tts/tts_per_rf/tts_per_rf_figs/Comparison_Table.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/scdrive2/TTS_2020/get_tts/tts_per_rf/tts_per_rf_figs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06ACA11-CC7C-F346-80AA-B45A28FF2094}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9C890C-60C9-684A-BC8C-AFA96E5DF14F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="22940" windowHeight="14260" xr2:uid="{A3DC752E-61BA-FC41-BD95-3822EA5ED517}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="troposphere tau" sheetId="1" r:id="rId1"/>
+    <sheet name="bl tau  " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
   <si>
     <t xml:space="preserve">Flight </t>
   </si>
@@ -73,6 +74,12 @@
   </si>
   <si>
     <t>Not Sorted</t>
+  </si>
+  <si>
+    <t>BL LIFETIME</t>
+  </si>
+  <si>
+    <t>TROPOSPHERE LIFETIME</t>
   </si>
 </sst>
 </file>
@@ -82,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,7 +99,22 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -140,19 +162,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,318 +491,667 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E466F8-008E-B84B-9055-2149322C7832}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>5.9</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.78</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="B4" s="5">
+        <v>2.6</v>
+      </c>
+      <c r="C4" s="5">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H4" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H3" s="2">
-        <v>2.1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2.1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.68</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="G6" s="5">
+        <v>2.6</v>
+      </c>
+      <c r="H6" s="5">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3.6</v>
+      </c>
+      <c r="C7" s="5">
+        <v>13.1</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.87</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="5">
         <v>2.8</v>
       </c>
-      <c r="I4" s="3">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="H7" s="5">
+        <v>10.3</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5">
         <v>2.8</v>
       </c>
-      <c r="D5" s="3">
-        <v>0.82</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="H5" s="2">
-        <v>5.9</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="C8" s="5">
+        <v>10.3</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>7.7</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="G8" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>11.9</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>11.9</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.88</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="5">
+        <v>3.6</v>
+      </c>
+      <c r="H9" s="5">
+        <v>13.1</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="C10" s="5">
+        <v>14.2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="H10" s="5">
+        <v>14.2</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C11" s="5">
+        <v>17.7</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.87</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="H11" s="5">
+        <v>14</v>
+      </c>
+      <c r="I11" s="6">
         <v>0.92</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="H6" s="2">
-        <v>6</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="C7" s="2">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.91</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="H7" s="2">
-        <v>7</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="C8" s="2">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.89</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="2">
-        <v>2</v>
-      </c>
-      <c r="H8" s="2">
-        <v>7.7</v>
-      </c>
-      <c r="I8" s="3">
+    </row>
+    <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="C12" s="5">
+        <v>14</v>
+      </c>
+      <c r="D12" s="6">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="E12" s="3"/>
+      <c r="F12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H12" s="5">
+        <v>17.7</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="C13" s="5">
+        <v>21.3</v>
+      </c>
+      <c r="D13" s="6">
         <v>0.92</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2">
-        <v>2</v>
-      </c>
-      <c r="H9" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="I9" s="3">
+      <c r="E13" s="3"/>
+      <c r="F13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="H13" s="5">
+        <v>21.3</v>
+      </c>
+      <c r="I13" s="6">
         <v>0.92</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2.8</v>
-      </c>
-      <c r="C10" s="2">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="2">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="H10" s="2">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C11" s="2">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.93</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="2">
-        <v>2.8</v>
-      </c>
-      <c r="H11" s="2">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2">
-        <v>11.9</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.93</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="2">
-        <v>3</v>
-      </c>
-      <c r="H12" s="2">
-        <v>11.9</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0.93</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="F3:I12">
-    <sortCondition ref="G2"/>
+  <sortState ref="F4:I13">
+    <sortCondition ref="G4"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5E0F95-1B47-E14A-93A2-C7B06914069C}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5.9</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.78</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.68</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2.8</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2.8</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.82</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5.9</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5">
+        <v>7.7</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.92</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="H7" s="5">
+        <v>6</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="C8" s="5">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.91</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="H8" s="5">
+        <v>7</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="C9" s="5">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="5">
+        <v>2</v>
+      </c>
+      <c r="H9" s="5">
+        <v>7.7</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2</v>
+      </c>
+      <c r="C10" s="5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.92</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="5">
+        <v>2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2.8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H11" s="5">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C12" s="5">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.93</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="5">
+        <v>2.8</v>
+      </c>
+      <c r="H12" s="5">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5">
+        <v>3</v>
+      </c>
+      <c r="C13" s="5">
+        <v>11.9</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.93</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="5">
+        <v>3</v>
+      </c>
+      <c r="H13" s="5">
+        <v>11.9</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>